<commit_message>
Formats the "Citation Gecko notebook" free text with maximum column width
</commit_message>
<xml_diff>
--- a/output/citation_gecko/Recommendations_wb_bak.xlsx
+++ b/output/citation_gecko/Recommendations_wb_bak.xlsx
@@ -1642,7 +1642,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>BÃ©guin, A. A.; Glas, C. A. W.</t>
+          <t>Béguin, A. A.; Glas, C. A. W.</t>
         </is>
       </c>
       <c r="B28">
@@ -1715,7 +1715,7 @@
       </c>
       <c r="AF28" t="inlineStr">
         <is>
-          <t>BÃ©guin y Glas - 2001 - MCMC estimation and some model-fit analysis of mul.pdf:C\:\\Users\\Mori.P16\\Zotero\\storage\\74ZAQMZ5\\BÃ©guin y Glas - 2001 - MCMC estimation and some model-fit analysis of mul.pdf:application/pdf</t>
+          <t>Béguin y Glas - 2001 - MCMC estimation and some model-fit analysis of mul.pdf:C\:\\Users\\Mori.P16\\Zotero\\storage\\74ZAQMZ5\\Béguin y Glas - 2001 - MCMC estimation and some model-fit analysis of mul.pdf:application/pdf</t>
         </is>
       </c>
     </row>
@@ -2575,7 +2575,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>â€œGuessingâ€  Parameter Estimates for Multidimensional Item Response Theory Models</t>
+          <t>“Guessing” Parameter Estimates for Multidimensional Item Response Theory Models</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -2600,7 +2600,7 @@
       </c>
       <c r="AF49" t="inlineStr">
         <is>
-          <t>DeMars - 2007 - â€œGuessingâ€  Parameter Estimates for Multidimensiona.pdf:C\:\\Users\\Mori.P16\\Zotero\\storage\\I8XZ8JU8\\DeMars - 2007 - â€œGuessingâ€  Parameter Estimates for Multidimensiona.pdf:application/pdf</t>
+          <t>DeMars - 2007 - “Guessing” Parameter Estimates for Multidimensiona.pdf:C\:\\Users\\Mori.P16\\Zotero\\storage\\I8XZ8JU8\\DeMars - 2007 - “Guessing” Parameter Estimates for Multidimensiona.pdf:application/pdf</t>
         </is>
       </c>
     </row>
@@ -3095,7 +3095,7 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Multidimensional Adaptive Testing with Kullbackâ€“Leibler Information Item Selection</t>
+          <t>Multidimensional Adaptive Testing with Kullback–Leibler Information Item Selection</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -3120,7 +3120,7 @@
       </c>
       <c r="AF62" t="inlineStr">
         <is>
-          <t>Mulder - 2009 - Multidimensional Adaptive Testing with Kullbackâ€“Le.pdf:C\:\\Users\\Mori.P16\\Zotero\\storage\\XG53VJFF\\Mulder - 2009 - Multidimensional Adaptive Testing with Kullbackâ€“Le.pdf:application/pdf</t>
+          <t>Mulder - 2009 - Multidimensional Adaptive Testing with Kullback–Le.pdf:C\:\\Users\\Mori.P16\\Zotero\\storage\\XG53VJFF\\Mulder - 2009 - Multidimensional Adaptive Testing with Kullback–Le.pdf:application/pdf</t>
         </is>
       </c>
     </row>
@@ -3415,7 +3415,7 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Kullbackâ€“Leibler Information and Its Applications in Multi-Dimensional Adaptive Testing</t>
+          <t>Kullback–Leibler Information and Its Applications in Multi-Dimensional Adaptive Testing</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -3440,7 +3440,7 @@
       </c>
       <c r="AF70" t="inlineStr">
         <is>
-          <t>Wang - 2011 - Kullbackâ€“Leibler Information and Its Applications .pdf:C\:\\Users\\Mori.P16\\Zotero\\storage\\WZ9QYXIN\\Wang - 2011 - Kullbackâ€“Leibler Information and Its Applications .pdf:application/pdf</t>
+          <t>Wang - 2011 - Kullback–Leibler Information and Its Applications .pdf:C\:\\Users\\Mori.P16\\Zotero\\storage\\WZ9QYXIN\\Wang - 2011 - Kullback–Leibler Information and Its Applications .pdf:application/pdf</t>
         </is>
       </c>
     </row>
@@ -3455,7 +3455,7 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Item Selection in Multidimensional Computerized Adaptive Testingâ€”Gaining Information from Different Angles</t>
+          <t>Item Selection in Multidimensional Computerized Adaptive Testing—Gaining Information from Different Angles</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -3885,7 +3885,7 @@
       </c>
       <c r="AG80" t="inlineStr">
         <is>
-          <t>Through simulated data, five multidimensional computerized adaptive testing (MCAT) selection procedures with varying test lengths are examined and compared using different stopping rules. Fixed item exposure rates are used for all the items, and the Priority Index (PI) method is used for the content constraints. Two stopping rules, standard error (SE) and predicted standard error reduction (PSER), are proposed; each MCAT selection process is stopped if either the required precision has been achieved or the selected number of items has reached the maximum limit. The five procedures are as follows: minimum angle (Ag), volume (Vm), minimize the error variance of the linear combination (V 1), minimize the error variance of the composite score with the optimized weight (V 2), and Kullbackâ€“Leibler (KL) information. The recovery for the domain scores or content scores and their overall score, test length, and test reliability are compared across the five MCAT procedures and between the two stopping rules. It is found that the two stopping rules are implemented successfully and that KL uses the least number of items to reach the same precision level, followed by Vm; Ag uses the largest number of items. On average, to reach a precision of SE = .35, 40, 55, 63, 63, and 82 items are needed for KL, Vm, V 1, V 2, and Ag, respectively, for the SE stopping rule. PSER yields 38, 45, 53, 58, and 68 items for KL, Vm, V 1, V 2, and Ag, respectively; PSER yields only slightly worse results than SE, but with much fewer items. Overall, KL is recommended for varying-length MCAT.</t>
+          <t>Through simulated data, five multidimensional computerized adaptive testing (MCAT) selection procedures with varying test lengths are examined and compared using different stopping rules. Fixed item exposure rates are used for all the items, and the Priority Index (PI) method is used for the content constraints. Two stopping rules, standard error (SE) and predicted standard error reduction (PSER), are proposed; each MCAT selection process is stopped if either the required precision has been achieved or the selected number of items has reached the maximum limit. The five procedures are as follows: minimum angle (Ag), volume (Vm), minimize the error variance of the linear combination (V 1), minimize the error variance of the composite score with the optimized weight (V 2), and Kullback–Leibler (KL) information. The recovery for the domain scores or content scores and their overall score, test length, and test reliability are compared across the five MCAT procedures and between the two stopping rules. It is found that the two stopping rules are implemented successfully and that KL uses the least number of items to reach the same precision level, followed by Vm; Ag uses the largest number of items. On average, to reach a precision of SE = .35, 40, 55, 63, 63, and 82 items are needed for KL, Vm, V 1, V 2, and Ag, respectively, for the SE stopping rule. PSER yields 38, 45, 53, 58, and 68 items for KL, Vm, V 1, V 2, and Ag, respectively; PSER yields only slightly worse results than SE, but with much fewer items. Overall, KL is recommended for varying-length MCAT.</t>
         </is>
       </c>
       <c r="AH80" t="inlineStr">
@@ -4252,7 +4252,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Piton-GonÃ§alves</t>
+          <t>Piton-Gonçalves</t>
         </is>
       </c>
       <c r="B90">
@@ -4260,12 +4260,12 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>Teste Adaptativo Computadorizado Multidimensional com propÃ³sitos educacionais: princÃ­pios e mÃ©todos</t>
+          <t>Teste Adaptativo Computadorizado Multidimensional com propósitos educacionais: princípios e métodos</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>Ensaio: AvaliaÃ§Ã£o e PolÃ­ticas PÃºblicas em EducaÃ§Ã£o</t>
+          <t>Ensaio: Avaliação e Políticas Públicas em Educação</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
@@ -4285,14 +4285,14 @@
       </c>
       <c r="AF90" t="inlineStr">
         <is>
-          <t>Piton-GonÃ§alves - 2015 - Teste Adaptativo Computadorizado Multidimensional .pdf:C\:\\Users\\Mori.P16\\Zotero\\storage\\9EEYWIPZ\\Piton-GonÃ§alves - 2015 - Teste Adaptativo Computadorizado Multidimensional .pdf:application/pdf</t>
+          <t>Piton-Gonçalves - 2015 - Teste Adaptativo Computadorizado Multidimensional .pdf:C\:\\Users\\Mori.P16\\Zotero\\storage\\9EEYWIPZ\\Piton-Gonçalves - 2015 - Teste Adaptativo Computadorizado Multidimensional .pdf:application/pdf</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>çŽ‹</t>
+          <t>王</t>
         </is>
       </c>
       <c r="B91">
@@ -4650,7 +4650,7 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>A logâ€ linear multidimensional Rasch model for captureâ€“recapture</t>
+          <t>A log‐linear multidimensional Rasch model for capture–recapture</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
@@ -4675,7 +4675,7 @@
       </c>
       <c r="AF100" t="inlineStr">
         <is>
-          <t>Pelle - 2016 - A logâ€ linear multidimensional Rasch model for capt.pdf:C\:\\Users\\Mori.P16\\Zotero\\storage\\JWHN8R2V\\Pelle - 2016 - A logâ€ linear multidimensional Rasch model for capt.pdf:application/pdf</t>
+          <t>Pelle - 2016 - A log‐linear multidimensional Rasch model for capt.pdf:C\:\\Users\\Mori.P16\\Zotero\\storage\\JWHN8R2V\\Pelle - 2016 - A log‐linear multidimensional Rasch model for capt.pdf:application/pdf</t>
         </is>
       </c>
     </row>
@@ -4810,7 +4810,7 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>A multidimensional IRT approach for dimensionality assessment of standardised studentsâ€™ tests in mathematics</t>
+          <t>A multidimensional IRT approach for dimensionality assessment of standardised students’ tests in mathematics</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
@@ -5095,7 +5095,7 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>GestÃ£o \&amp; ProduÃ§Ã£o</t>
+          <t>Gestão \&amp; Produção</t>
         </is>
       </c>
       <c r="E111" t="inlineStr">
@@ -5242,7 +5242,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>ÅžahiÌ‡n, Sakine GÃ–Ã‡ER; Eser, Derya Ã‡AKICI; Gelbal, Selahattin</t>
+          <t>Şahi̇n, Sakine GÖÇER; Eser, Derya ÇAKICI; Gelbal, Selahattin</t>
         </is>
       </c>
       <c r="B115">
@@ -5310,12 +5310,12 @@
       </c>
       <c r="AF115" t="inlineStr">
         <is>
-          <t>ÅžahiÌ‡n et al. - 2018 - The Interaction Effect of the Correlation between .pdf:C\:\\Users\\Mori.P16\\Zotero\\storage\\JT54ZPZQ\\ÅžahiÌ‡n et al. - 2018 - The Interaction Effect of the Correlation between .pdf:application/pdf</t>
+          <t>Şahi̇n et al. - 2018 - The Interaction Effect of the Correlation between .pdf:C\:\\Users\\Mori.P16\\Zotero\\storage\\JT54ZPZQ\\Şahi̇n et al. - 2018 - The Interaction Effect of the Correlation between .pdf:application/pdf</t>
         </is>
       </c>
       <c r="AG115" t="inlineStr">
         <is>
-          <t>There are some studies in the literature that have considered the impact of modeling multidimensional mixed structured tests as unidimensional. These studies have demonstrated that the error associated with the discrimination parameters increases as the correlation between dimensions increases. In this study, the interaction between itemsâ€™ angles on coordinate system and the correlations between dimensions was investigated when estimating multidimensional tests as unidimensional. Data were simulated based on two dimensional, and two-parameter compensatory MIRT model. Angles of items were determined as 0. 15 o ; 0.30 o ; 0.45 o ; 0.60 o and 0.75 o respectively. The correlations between ability parameters were set to 0.15, 0.30, 0.45, 0.60 and 0.75 respectively, which are same with the angles of discrimination parameters. The ability distributions were generated from standard normal, positively and negatively skewed distributions. A total of 75 (5 x 5 x 3) conditions were studied: five different conditions for the correlation between dimensions; five different angles of items and three different ability distributions. For all conditions, the number of items was fixed at 25 and the sample size was fixed at n = 2,000. Item and ability parameter estimation were conducted using BILOG. For each condition, 100 replications were performed. The RMSE statistic was used to evaluate parameter estimation errors, when multidimensional response data were scaled using a unidimensional IRT model. Based on the findings, it can be concluded that the pattern of RMSE values especially for discrimination parameters are different from the existing studies in the literature in which multidimensional tests were estimated as unidimensional.</t>
+          <t>There are some studies in the literature that have considered the impact of modeling multidimensional mixed structured tests as unidimensional. These studies have demonstrated that the error associated with the discrimination parameters increases as the correlation between dimensions increases. In this study, the interaction between items’ angles on coordinate system and the correlations between dimensions was investigated when estimating multidimensional tests as unidimensional. Data were simulated based on two dimensional, and two-parameter compensatory MIRT model. Angles of items were determined as 0. 15 o ; 0.30 o ; 0.45 o ; 0.60 o and 0.75 o respectively. The correlations between ability parameters were set to 0.15, 0.30, 0.45, 0.60 and 0.75 respectively, which are same with the angles of discrimination parameters. The ability distributions were generated from standard normal, positively and negatively skewed distributions. A total of 75 (5 x 5 x 3) conditions were studied: five different conditions for the correlation between dimensions; five different angles of items and three different ability distributions. For all conditions, the number of items was fixed at 25 and the sample size was fixed at n = 2,000. Item and ability parameter estimation were conducted using BILOG. For each condition, 100 replications were performed. The RMSE statistic was used to evaluate parameter estimation errors, when multidimensional response data were scaled using a unidimensional IRT model. Based on the findings, it can be concluded that the pattern of RMSE values especially for discrimination parameters are different from the existing studies in the literature in which multidimensional tests were estimated as unidimensional.</t>
         </is>
       </c>
       <c r="AH115" t="inlineStr">
@@ -5695,7 +5695,7 @@
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>Multidimensional Test Assembly Using Mixed-Integer Linear Programming: An Application of Kullbackâ€“Leibler Information</t>
+          <t>Multidimensional Test Assembly Using Mixed-Integer Linear Programming: An Application of Kullback–Leibler Information</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">

</xml_diff>